<commit_message>
[RFT] Code improvements, comments, and tests
Code improvements to increase performance. Additional tests and
comments.

refs KIME-4583
</commit_message>
<xml_diff>
--- a/Tests/Functional/Fixtures/Resources/sample.xlsx
+++ b/Tests/Functional/Fixtures/Resources/sample.xlsx
@@ -15,17 +15,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>firstname</t>
+  </si>
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>lastname</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>ort</t>
+  </si>
+  <si>
     <t>Hans</t>
   </si>
   <si>
@@ -35,6 +41,9 @@
     <t>001</t>
   </si>
   <si>
+    <t>Zurich</t>
+  </si>
+  <si>
     <t>Simon</t>
   </si>
   <si>
@@ -42,6 +51,12 @@
   </si>
   <si>
     <t>002</t>
+  </si>
+  <si>
+    <t>Web Essentials</t>
+  </si>
+  <si>
+    <t>Phnom Penh</t>
   </si>
 </sst>
 </file>
@@ -122,7 +137,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -143,17 +158,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -166,27 +179,42 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>